<commit_message>
fix seed rules and users show bug
</commit_message>
<xml_diff>
--- a/db/school_info/project.xlsx
+++ b/db/school_info/project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a_flying_fish\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7540F4AA-B9D0-4C3F-B7EC-75282F932C68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD9D673-1AD3-4769-9A97-C049F565BA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2568" yWindow="2316" windowWidth="17280" windowHeight="8964" xr2:uid="{6042ADC9-6B9A-48A1-8D96-495469671B06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6042ADC9-6B9A-48A1-8D96-495469671B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>哲学</t>
   </si>
@@ -183,6 +183,35 @@
   <si>
     <t>一级学科</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
   </si>
 </sst>
 </file>
@@ -235,18 +264,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,96 +597,97 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
+    <col min="1" max="1" width="8.88671875" style="3"/>
     <col min="2" max="2" width="69.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1">
+    <row r="1" spans="1:2" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -662,7 +695,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -670,7 +703,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -678,7 +711,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -686,7 +719,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -694,7 +727,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -702,7 +735,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -710,7 +743,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -718,7 +751,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -726,7 +759,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -734,7 +767,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -742,7 +775,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -750,7 +783,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -758,7 +791,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -766,7 +799,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -774,7 +807,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -782,7 +815,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -790,7 +823,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -798,7 +831,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -806,7 +839,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -814,7 +847,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -822,7 +855,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -830,7 +863,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -838,7 +871,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -846,7 +879,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -854,7 +887,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -862,7 +895,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -870,7 +903,7 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -878,7 +911,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" t="s">
@@ -886,7 +919,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -894,7 +927,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -902,7 +935,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -910,7 +943,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -918,7 +951,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -926,7 +959,7 @@
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -934,7 +967,7 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" t="s">
@@ -942,7 +975,7 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" t="s">
@@ -950,7 +983,7 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" t="s">
@@ -958,8 +991,8 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="22.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>